<commit_message>
Admin dashboard: filters for recent orders (결제완료/입금전), updated stats/cards and icons, recent activity scrolling + date spacing; InquiryManagement: default right panel closed, mobile send button, email-only author, UI tweaks; tailwind animations; misc fixes
</commit_message>
<xml_diff>
--- a/수정사항_애드모어.xlsx
+++ b/수정사항_애드모어.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seoinjeong/Library/Mobile Documents/com~apple~CloudDocs/0. 프로젝트/ADMore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1BF852-71ED-B844-B5B1-32895E3696EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA3CAC3-22DD-B84C-B022-086AF5B73CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41320" yWindow="500" windowWidth="27680" windowHeight="19220" xr2:uid="{812FD805-9A5A-E843-B914-C38D28068475}"/>
+    <workbookView xWindow="-21880" yWindow="3540" windowWidth="21860" windowHeight="18060" xr2:uid="{812FD805-9A5A-E843-B914-C38D28068475}"/>
   </bookViews>
   <sheets>
     <sheet name="나중에 수정할것" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -415,6 +415,14 @@
   </si>
   <si>
     <t>실제로 최근에 본상품이 아님</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문관리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제내역 클릭후 모달로 나오는 폼 수정하기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1025,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51ACB9AF-9FC2-C748-AD7B-775CDB889580}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1172,55 +1180,58 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" t="s">
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
       <c r="C23" t="s">
         <v>71</v>
       </c>
       <c r="D23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
-      <c r="D24" t="s">
+    <row r="25" spans="2:5">
+      <c r="D25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="38">
-      <c r="B26" t="s">
+    <row r="27" spans="2:5" ht="38">
+      <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="C27" t="s">
+    <row r="28" spans="2:5">
+      <c r="C28" t="s">
         <v>77</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -1228,25 +1239,33 @@
         <v>56</v>
       </c>
       <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" t="s">
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
         <v>74</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>85</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
-      <c r="C33" t="s">
+    <row r="34" spans="2:4">
+      <c r="C34" t="s">
         <v>87</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>